<commit_message>
Uklanjanje nepotrebnih redova u tabeli
</commit_message>
<xml_diff>
--- a/IzlazakSaAutoputa/testovi.xlsx
+++ b/IzlazakSaAutoputa/testovi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -208,13 +208,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,7 +258,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -441,19 +448,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
@@ -463,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -486,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -498,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,20 +507,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,114 +972,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="21">
         <v>42756</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>